<commit_message>
testd by jackwang in Cathy's laptop
</commit_message>
<xml_diff>
--- a/data/testcase.xlsx
+++ b/data/testcase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17655"/>
+    <workbookView windowWidth="18600" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>描述</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>user=wangbo&amp;pwd=1234567</t>
+  </si>
+  <si>
+    <t>updated at 2024-04-17 by Cathy's laptop</t>
+  </si>
+  <si>
+    <t>login_api_003</t>
   </si>
 </sst>
 </file>
@@ -1033,10 +1039,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
-    <col min="2" max="2" width="18.375" customWidth="1"/>
-    <col min="3" max="3" width="46.5" customWidth="1"/>
-    <col min="5" max="5" width="25.875" customWidth="1"/>
+    <col min="1" max="1" width="47.0619469026549" customWidth="1"/>
+    <col min="2" max="2" width="18.3716814159292" customWidth="1"/>
+    <col min="3" max="3" width="46.5044247787611" customWidth="1"/>
+    <col min="5" max="5" width="25.8761061946903" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1096,8 +1102,12 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>

</xml_diff>